<commit_message>
Added new metadata file
</commit_message>
<xml_diff>
--- a/meta/proj_B-101-533__MetaData_04_11_2023.xlsx
+++ b/meta/proj_B-101-533__MetaData_04_11_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/elkriefa_mskcc_org/Documents/!GDriveMigratedData/My Documents/ladanyi_lab/in_prep/colitis_data/case_lists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/IGNIS/juno/work/bic/socci/Work/Users/PeledJ/ElkriefA/Proj_B-101-533/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DD2DBE0-A765-8647-8AA9-A71308A68755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB68CFAB-8C94-894C-9566-379D5C4636DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="3160" windowWidth="39000" windowHeight="21680" activeTab="1" xr2:uid="{EDF77AB5-CA95-1C4A-94FB-8885432FCC05}"/>
+    <workbookView xWindow="12200" yWindow="3160" windowWidth="39000" windowHeight="24660" xr2:uid="{EDF77AB5-CA95-1C4A-94FB-8885432FCC05}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotypes" sheetId="1" r:id="rId1"/>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADF492F-4596-A340-8243-222099F24153}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EA950A-93C5-A14B-B2E8-CCF5C5A4CE98}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28" x14ac:dyDescent="0.3"/>

</xml_diff>